<commit_message>
nuevo direccionamiento de inventario, y planilla
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/trabajadores.xlsx
+++ b/ProyectoPooDist/excels/trabajadores.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Nombre</t>
   </si>
@@ -56,11 +56,25 @@
 sumamente alto</t>
   </si>
   <si>
-    <t>Emma Myers</t>
+    <t xml:space="preserve">Emma </t>
   </si>
   <si>
     <t>Encarga de relaciones externas
 Sumamente talentosa</t>
+  </si>
+  <si>
+    <t>Trabajador de ejemplo</t>
+  </si>
+  <si>
+    <t>descripcion
+de
+ejemplo</t>
+  </si>
+  <si>
+    <t>hola como estas</t>
+  </si>
+  <si>
+    <t>mu bien</t>
   </si>
 </sst>
 </file>
@@ -105,7 +119,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -209,6 +223,32 @@
         <v>600.0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>600.0</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="F5" t="n" s="0">
+        <v>-123.0</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H5" t="n" s="0">
+        <v>456.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>